<commit_message>
Correção da escrita dos dados no documento excel e imprimindo os dados no formato JSON no end-point users
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,10 +434,22 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="n">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
         <v>1</v>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B2" t="inlineStr">
         <is>
           <t>Emerson</t>
         </is>

</xml_diff>